<commit_message>
modified:   DANL340/Origin/md_crime.xlsx modified:   DANL340/Test4.ipynb new file:   DANL470/Attempt_MM1.xlsx new file:   DANL470/Attempt_MM2.xlsx new file:   DANL470/Attempt_MM3.xlsx new file:   DANL470/Attempt_MM4.xlsx new file:   DANL470/Attempt_MM5.xlsx new file:   DANL470/Project4.ipynb modified:   Lab6/Lab6.ipynb
</commit_message>
<xml_diff>
--- a/DANL340/Origin/md_crime.xlsx
+++ b/DANL340/Origin/md_crime.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DANL340\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silen\HealthDataAnalytics\DANL340\Origin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0598F1F0-C7D8-40C2-A432-7CF2BBBE70D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A32C90-A092-4367-962E-A7DAFF48FCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,10 +152,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +472,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -514,7 +513,7 @@
       <c r="E2" s="1">
         <v>1529</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -534,7 +533,7 @@
       <c r="E3" s="1">
         <v>10433</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>3</v>
       </c>
     </row>
@@ -554,7 +553,7 @@
       <c r="E4" s="1">
         <v>28147</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>5</v>
       </c>
     </row>
@@ -574,7 +573,7 @@
       <c r="E5" s="1">
         <v>20045</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>8</v>
       </c>
     </row>
@@ -594,7 +593,7 @@
       <c r="E6" s="1">
         <v>866</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>2</v>
       </c>
     </row>
@@ -614,7 +613,7 @@
       <c r="E7" s="1">
         <v>459</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>0</v>
       </c>
     </row>
@@ -634,7 +633,7 @@
       <c r="E8" s="1">
         <v>1373</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>0</v>
       </c>
     </row>
@@ -654,7 +653,7 @@
       <c r="E9" s="1">
         <v>2027</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>1</v>
       </c>
     </row>
@@ -674,7 +673,7 @@
       <c r="E10" s="1">
         <v>2669</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>2</v>
       </c>
     </row>
@@ -694,7 +693,7 @@
       <c r="E11" s="1">
         <v>982</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>1</v>
       </c>
     </row>
@@ -714,7 +713,7 @@
       <c r="E12" s="1">
         <v>2671</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>2</v>
       </c>
     </row>
@@ -734,7 +733,7 @@
       <c r="E13" s="1">
         <v>357</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>0</v>
       </c>
     </row>
@@ -754,7 +753,7 @@
       <c r="E14" s="1">
         <v>2217</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>2</v>
       </c>
     </row>
@@ -774,7 +773,7 @@
       <c r="E15" s="1">
         <v>3993</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>1</v>
       </c>
     </row>
@@ -794,7 +793,7 @@
       <c r="E16" s="1">
         <v>152</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>0</v>
       </c>
     </row>
@@ -814,7 +813,7 @@
       <c r="E17" s="1">
         <v>16594</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>3</v>
       </c>
     </row>
@@ -834,7 +833,7 @@
       <c r="E18" s="1">
         <v>19401</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>1</v>
       </c>
     </row>
@@ -854,7 +853,7 @@
       <c r="E19" s="1">
         <v>437</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>0</v>
       </c>
     </row>
@@ -874,7 +873,7 @@
       <c r="E20" s="1">
         <v>398</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>0</v>
       </c>
     </row>
@@ -894,7 +893,7 @@
       <c r="E21" s="1">
         <v>1744</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>0</v>
       </c>
     </row>
@@ -914,7 +913,7 @@
       <c r="E22" s="1">
         <v>477</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>0</v>
       </c>
     </row>
@@ -934,7 +933,7 @@
       <c r="E23" s="1">
         <v>2249</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>1</v>
       </c>
     </row>
@@ -954,7 +953,7 @@
       <c r="E24" s="1">
         <v>2202</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>0</v>
       </c>
     </row>
@@ -974,7 +973,7 @@
       <c r="E25" s="1">
         <v>1536</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>